<commit_message>
Fixed huefner, ellwangen, goldbeck, heidelberg
</commit_message>
<xml_diff>
--- a/tests/converters/data/huefner.xlsx
+++ b/tests/converters/data/huefner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTL\FTLBank\ipl\data\xlsx\huefner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTL\FTLBank\ipl\data\IPL_ParkAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAA9D8D-1975-4F3A-A437-2ED9AE329FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF0A982-7A7C-470E-BA19-4B4B69A7B382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="245">
   <si>
     <t>Dokumentation (statische) Parkdaten-Import-Tabelle</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t>06:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja </t>
   </si>
 </sst>
 </file>
@@ -1746,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1900,7 +1903,7 @@
         <v>68</v>
       </c>
       <c r="O2" t="s">
-        <v>68</v>
+        <v>244</v>
       </c>
       <c r="P2" t="s">
         <v>69</v>
@@ -3647,6 +3650,9 @@
       </c>
       <c r="G38" t="s">
         <v>148</v>
+      </c>
+      <c r="I38">
+        <v>166</v>
       </c>
       <c r="N38" t="s">
         <v>68</v>
@@ -7384,15 +7390,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010065FFA48B2CE5744C9996928006727830" ma:contentTypeVersion="18" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="1501545ff204d846336c3ec87f72a2f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c90a47bc-c666-4794-b410-4f922560bad8" xmlns:ns3="e217ae6d-b740-4417-8c03-3a632d5383d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e5dc165aee6c71002a08fdc37524b31" ns2:_="" ns3:_="">
     <xsd:import namespace="c90a47bc-c666-4794-b410-4f922560bad8"/>
@@ -7647,6 +7644,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7659,14 +7665,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A744213D-2345-411A-8075-D563A27669AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{341A3ECC-777C-45FC-80F7-7B2B5AEE7C41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7681,6 +7679,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A744213D-2345-411A-8075-D563A27669AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>